<commit_message>
para la seniora p
</commit_message>
<xml_diff>
--- a/TP2/1.Datos/LC.xlsx
+++ b/TP2/1.Datos/LC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OperaDownload\Laboratorio Electronica\lab-electronica\TP2\1.Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BA4317-0A32-4E50-A3E0-AE4D2DCA9820}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D2734F-809F-4B59-919E-4D44D89D37E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" activeTab="1" xr2:uid="{E00BE3E8-5786-4D69-AFA6-9A9995C46107}"/>
   </bookViews>
@@ -1819,8 +1819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C48A329-5B62-4B04-8CE8-D5F7ABFEC796}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2566,54 +2566,54 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>10000000</v>
+        <v>9000000</v>
       </c>
       <c r="B31" s="1">
-        <v>2.2999999999999998</v>
+        <v>1.6</v>
       </c>
       <c r="C31">
-        <v>85.95</v>
+        <v>84.16</v>
       </c>
       <c r="D31">
-        <v>0.16</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="E31" s="1">
-        <v>3.6360000000000003E-8</v>
+        <v>2.7999999999999999E-8</v>
       </c>
       <c r="F31" s="1">
-        <v>6.9699999999999997E-9</v>
+        <v>1.111E-8</v>
       </c>
       <c r="G31">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H31">
-        <v>7.0000000000000007E-2</v>
+        <v>0.10199999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>9000000</v>
+        <v>10000000</v>
       </c>
       <c r="B32" s="1">
-        <v>1.6</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C32">
-        <v>84.16</v>
+        <v>85.95</v>
       </c>
       <c r="D32">
-        <v>0.16200000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="E32" s="1">
-        <v>2.7999999999999999E-8</v>
+        <v>3.6360000000000003E-8</v>
       </c>
       <c r="F32" s="1">
-        <v>1.111E-8</v>
+        <v>6.9699999999999997E-9</v>
       </c>
       <c r="G32">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H32">
-        <v>0.10199999999999999</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>